<commit_message>
add hoard bonus (coins)
</commit_message>
<xml_diff>
--- a/dd5-generator/src/treasureGenerator/files/hoardGen.xlsx
+++ b/dd5-generator/src/treasureGenerator/files/hoardGen.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DDGen\DD5Generator\dd5-generator\src\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\Documents\DEV\DnD\DD5-Generator\dd5-generator\src\treasureGenerator\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E134F3-17DA-4047-8776-003F9B5D98CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EB21BD-9A82-49B1-8971-F2C391748277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="BONUS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>1d20</t>
   </si>
@@ -136,6 +137,24 @@
   </si>
   <si>
     <t>10-13</t>
+  </si>
+  <si>
+    <t>5d6 × 100 (1700) pa 2d4 × 10 (50) po</t>
+  </si>
+  <si>
+    <t>1d6 × 1000 (3500) pa 3d6 × 100 (1050) po 1d6 × 10 (35) pp</t>
+  </si>
+  <si>
+    <t>BONUS</t>
+  </si>
+  <si>
+    <t>2d6 × 1000 (7000) pa 6d6 × 100 (2100) po 3d6 × 10 (105) pp</t>
+  </si>
+  <si>
+    <t>4d6 × 1000 (14000) po 5d6 × 100 (1750) pp</t>
+  </si>
+  <si>
+    <t>12d6 × 1000 (42000) po 8d6 × 1000 (28000) pp</t>
   </si>
 </sst>
 </file>
@@ -205,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -227,6 +246,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,21 +532,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -544,7 +566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
@@ -564,7 +586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>34</v>
       </c>
@@ -584,7 +606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>35</v>
       </c>
@@ -604,7 +626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -624,7 +646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -644,7 +666,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -664,7 +686,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>20</v>
       </c>
@@ -688,4 +710,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351C4380-5E80-447D-AB3E-26F79935CE37}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="4" width="50.5703125" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>